<commit_message>
added saving records to the database
</commit_message>
<xml_diff>
--- a/Data/Result/result.xlsx
+++ b/Data/Result/result.xlsx
@@ -33,25 +33,13 @@
     <t>Владивосток</t>
   </si>
   <si>
-    <t>Воронеж</t>
+    <t>Москва_x000d_</t>
   </si>
   <si>
     <t>Максимальная температура</t>
   </si>
   <si>
-    <t>Иркутск</t>
-  </si>
-  <si>
-    <t>Москва</t>
-  </si>
-  <si>
     <t>Минимальная температура</t>
-  </si>
-  <si>
-    <t>Новосибирск</t>
-  </si>
-  <si>
-    <t>Чита</t>
   </si>
 </sst>
 </file>
@@ -168,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -185,20 +173,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -207,19 +201,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -276,52 +261,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Температура городов'!$B$3:$B$8</c:f>
+              <c:f>'Температура городов'!$B$3:$B$4</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Владивосток</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Воронеж</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Иркутск</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Москва</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Новосибирск</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Чита</c:v>
+                  <c:v>Москва
+</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Температура городов'!$C$3:$C$8</c:f>
+              <c:f>'Температура городов'!$C$3:$C$4</c:f>
               <c:numCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -739,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="4">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -747,7 +709,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="6">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -756,111 +718,95 @@
         <v>4</v>
       </c>
       <c r="C4" s="8">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="10">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="11"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8">
-        <v>25</v>
-      </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6">
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="11">
-        <v>28</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="13">
-        <v>20</v>
+      <c r="F6" s="15">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8">
-        <v>26</v>
-      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="7"/>
     </row>
     <row r="8">
-      <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="6">
-        <v>22</v>
-      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="7"/>
     </row>
     <row r="9">
-      <c r="B9" s="12"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="7"/>
     </row>
     <row r="10">
-      <c r="B10" s="12"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="7"/>
     </row>
     <row r="11">
-      <c r="B11" s="12"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="7"/>
     </row>
     <row r="12">
-      <c r="B12" s="12"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="7"/>
     </row>
     <row r="13">
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="7"/>
     </row>
     <row r="14">
-      <c r="B14" s="18"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="7"/>
     </row>
     <row r="15">
-      <c r="B15" s="18"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="7"/>
     </row>
     <row r="16">
-      <c r="B16" s="18"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="7"/>
     </row>
     <row r="17">
-      <c r="B17" s="18"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="7"/>
     </row>
     <row r="18">
-      <c r="B18" s="18"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19">
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
     </row>
   </sheetData>
   <pageSetup r:id="rId1" paperSize="9" orientation="portrait"/>
@@ -888,44 +834,44 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5">
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6">
-      <c r="B6" s="20"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
     </row>
     <row r="7">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
     </row>
     <row r="8">
-      <c r="B8" s="20"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
     </row>
     <row r="9">
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
     </row>
     <row r="10">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>